<commit_message>
Misc bug fixes, add summary tables
</commit_message>
<xml_diff>
--- a/results/sensitivity_vs_error.xlsx
+++ b/results/sensitivity_vs_error.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\reseek_scop40\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A288D16-F61B-4455-BD96-22B19AF3EB27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC6249A-4B04-444C-93BE-441F9BBF415E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11160" yWindow="2580" windowWidth="24945" windowHeight="15900" activeTab="2" xr2:uid="{30A151E1-5A68-4C81-B266-04173DADF783}"/>
+    <workbookView xWindow="11355" yWindow="2430" windowWidth="26460" windowHeight="15900" activeTab="2" xr2:uid="{30A151E1-5A68-4C81-B266-04173DADF783}"/>
   </bookViews>
   <sheets>
     <sheet name="Ignore" sheetId="2" r:id="rId1"/>

</xml_diff>

<commit_message>
Various fixes and re-runs, now reseek C++ and reseek_scop40 python accuracy agrees
</commit_message>
<xml_diff>
--- a/results/sensitivity_vs_error.xlsx
+++ b/results/sensitivity_vs_error.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\reseek_scop40\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26C8D2E-8178-45FF-96A3-E1218461EC9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237B7E8D-77D6-4AAC-ACAD-5E751D62312D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2970" yWindow="2070" windowWidth="29190" windowHeight="16125" xr2:uid="{30A151E1-5A68-4C81-B266-04173DADF783}"/>
+    <workbookView xWindow="3450" yWindow="2280" windowWidth="27720" windowHeight="15615" activeTab="2" xr2:uid="{30A151E1-5A68-4C81-B266-04173DADF783}"/>
   </bookViews>
   <sheets>
     <sheet name="Ignore" sheetId="2" r:id="rId1"/>
@@ -12117,16 +12117,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12559,7 +12559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9E49264-24AA-4A3A-8626-19F8BEE0B881}">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14978,7 +14978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA24BEAF-4687-47A5-8CF2-B3CF9CEEAC51}">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Remove obsolete reseek-sensitive results
</commit_message>
<xml_diff>
--- a/results/sensitivity_vs_error.xlsx
+++ b/results/sensitivity_vs_error.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\reseek_scop40\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8AE384-BC14-4D45-91D3-C60305BC66C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32B2073-B9E8-46DB-9DB0-71ED9C91922F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{30A151E1-5A68-4C81-B266-04173DADF783}"/>
   </bookViews>
@@ -1037,115 +1037,112 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="43"/>
                 <c:pt idx="5">
-                  <c:v>1.516E-2</c:v>
+                  <c:v>1.5339999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.614E-2</c:v>
+                  <c:v>2.266E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.916E-2</c:v>
+                  <c:v>3.3000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.0569999999999999E-2</c:v>
+                  <c:v>4.6829999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.7410000000000002E-2</c:v>
+                  <c:v>6.1190000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1202</c:v>
+                  <c:v>8.1079999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.16489999999999999</c:v>
+                  <c:v>0.1046</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.21029999999999999</c:v>
+                  <c:v>0.12870000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.2671</c:v>
+                  <c:v>0.15790000000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.33400000000000002</c:v>
+                  <c:v>0.1946</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.41920000000000002</c:v>
+                  <c:v>0.23680000000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.51439999999999997</c:v>
+                  <c:v>0.28460000000000002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.61539999999999995</c:v>
+                  <c:v>0.34079999999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.7379</c:v>
+                  <c:v>0.40810000000000002</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.88560000000000005</c:v>
+                  <c:v>0.4899</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.038</c:v>
+                  <c:v>0.57689999999999997</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.2130000000000001</c:v>
+                  <c:v>0.68110000000000004</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.403</c:v>
+                  <c:v>0.81289999999999996</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.599</c:v>
+                  <c:v>0.95940000000000003</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.821</c:v>
+                  <c:v>1.1279999999999999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.0529999999999999</c:v>
+                  <c:v>1.3340000000000001</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.2989999999999999</c:v>
+                  <c:v>1.548</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.581</c:v>
+                  <c:v>1.7929999999999999</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.8889999999999998</c:v>
+                  <c:v>2.08</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.218</c:v>
+                  <c:v>2.4009999999999998</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.556</c:v>
+                  <c:v>2.7679999999999998</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.9249999999999998</c:v>
+                  <c:v>3.1880000000000002</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.3259999999999996</c:v>
+                  <c:v>3.6619999999999999</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4.7690000000000001</c:v>
+                  <c:v>4.1689999999999996</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>5.24</c:v>
+                  <c:v>4.7380000000000004</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>5.7439999999999998</c:v>
+                  <c:v>5.3369999999999997</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>6.3239999999999998</c:v>
+                  <c:v>5.9909999999999997</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>6.9089999999999998</c:v>
+                  <c:v>6.7069999999999999</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>7.54</c:v>
+                  <c:v>7.4509999999999996</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>8.2479999999999993</c:v>
+                  <c:v>8.266</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>9.0210000000000008</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>9.8529999999999998</c:v>
+                  <c:v>9.1129999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5282,10 +5279,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D48A558-673B-4B1E-8FF7-FCB07FA6F0FA}">
-  <dimension ref="A1:G87"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X31" sqref="X31"/>
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5367,7 +5364,7 @@
         <v>1.222E-2</v>
       </c>
       <c r="G7">
-        <v>1.516E-2</v>
+        <v>1.5339999999999999E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -5384,7 +5381,7 @@
         <v>2.3640000000000001E-2</v>
       </c>
       <c r="G8">
-        <v>2.614E-2</v>
+        <v>2.266E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -5404,7 +5401,7 @@
         <v>3.9600000000000003E-2</v>
       </c>
       <c r="G9">
-        <v>3.916E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -5424,7 +5421,7 @@
         <v>6.012E-2</v>
       </c>
       <c r="G10">
-        <v>6.0569999999999999E-2</v>
+        <v>4.6829999999999997E-2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -5447,7 +5444,7 @@
         <v>1.472E-2</v>
       </c>
       <c r="G11">
-        <v>8.7410000000000002E-2</v>
+        <v>6.1190000000000001E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -5470,7 +5467,7 @@
         <v>2.3910000000000001E-2</v>
       </c>
       <c r="G12">
-        <v>0.1202</v>
+        <v>8.1079999999999999E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -5493,7 +5490,7 @@
         <v>3.202E-2</v>
       </c>
       <c r="G13">
-        <v>0.16489999999999999</v>
+        <v>0.1046</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -5513,7 +5510,7 @@
         <v>4.5400000000000003E-2</v>
       </c>
       <c r="G14">
-        <v>0.21029999999999999</v>
+        <v>0.12870000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -5533,7 +5530,7 @@
         <v>6.0650000000000003E-2</v>
       </c>
       <c r="G15">
-        <v>0.2671</v>
+        <v>0.15790000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -5553,7 +5550,7 @@
         <v>7.9920000000000005E-2</v>
       </c>
       <c r="G16">
-        <v>0.33400000000000002</v>
+        <v>0.1946</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -5573,7 +5570,7 @@
         <v>0.1031</v>
       </c>
       <c r="G17">
-        <v>0.41920000000000002</v>
+        <v>0.23680000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -5593,7 +5590,7 @@
         <v>0.1308</v>
       </c>
       <c r="G18">
-        <v>0.51439999999999997</v>
+        <v>0.28460000000000002</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -5613,7 +5610,7 @@
         <v>0.1646</v>
       </c>
       <c r="G19">
-        <v>0.61539999999999995</v>
+        <v>0.34079999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -5633,7 +5630,7 @@
         <v>0.20680000000000001</v>
       </c>
       <c r="G20">
-        <v>0.7379</v>
+        <v>0.40810000000000002</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -5653,7 +5650,7 @@
         <v>0.26140000000000002</v>
       </c>
       <c r="G21">
-        <v>0.88560000000000005</v>
+        <v>0.4899</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -5673,7 +5670,7 @@
         <v>0.31859999999999999</v>
       </c>
       <c r="G22">
-        <v>1.038</v>
+        <v>0.57689999999999997</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -5693,7 +5690,7 @@
         <v>0.38900000000000001</v>
       </c>
       <c r="G23">
-        <v>1.2130000000000001</v>
+        <v>0.68110000000000004</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -5713,7 +5710,7 @@
         <v>0.47089999999999999</v>
       </c>
       <c r="G24">
-        <v>1.403</v>
+        <v>0.81289999999999996</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -5733,7 +5730,7 @@
         <v>0.56610000000000005</v>
       </c>
       <c r="G25">
-        <v>1.599</v>
+        <v>0.95940000000000003</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -5753,7 +5750,7 @@
         <v>0.68659999999999999</v>
       </c>
       <c r="G26">
-        <v>1.821</v>
+        <v>1.1279999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -5773,7 +5770,7 @@
         <v>0.83130000000000004</v>
       </c>
       <c r="G27">
-        <v>2.0529999999999999</v>
+        <v>1.3340000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -5793,7 +5790,7 @@
         <v>1.002</v>
       </c>
       <c r="G28">
-        <v>2.2989999999999999</v>
+        <v>1.548</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -5813,7 +5810,7 @@
         <v>1.204</v>
       </c>
       <c r="G29">
-        <v>2.581</v>
+        <v>1.7929999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -5833,7 +5830,7 @@
         <v>1.4319999999999999</v>
       </c>
       <c r="G30">
-        <v>2.8889999999999998</v>
+        <v>2.08</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -5853,7 +5850,7 @@
         <v>1.704</v>
       </c>
       <c r="G31">
-        <v>3.218</v>
+        <v>2.4009999999999998</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -5873,7 +5870,7 @@
         <v>2.0009999999999999</v>
       </c>
       <c r="G32">
-        <v>3.556</v>
+        <v>2.7679999999999998</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -5893,7 +5890,7 @@
         <v>2.34</v>
       </c>
       <c r="G33">
-        <v>3.9249999999999998</v>
+        <v>3.1880000000000002</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -5913,7 +5910,7 @@
         <v>2.7370000000000001</v>
       </c>
       <c r="G34">
-        <v>4.3259999999999996</v>
+        <v>3.6619999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -5933,7 +5930,7 @@
         <v>3.1989999999999998</v>
       </c>
       <c r="G35">
-        <v>4.7690000000000001</v>
+        <v>4.1689999999999996</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -5953,7 +5950,7 @@
         <v>3.7120000000000002</v>
       </c>
       <c r="G36">
-        <v>5.24</v>
+        <v>4.7380000000000004</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -5973,7 +5970,7 @@
         <v>4.3129999999999997</v>
       </c>
       <c r="G37">
-        <v>5.7439999999999998</v>
+        <v>5.3369999999999997</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -5993,7 +5990,7 @@
         <v>5.0250000000000004</v>
       </c>
       <c r="G38">
-        <v>6.3239999999999998</v>
+        <v>5.9909999999999997</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -6013,7 +6010,7 @@
         <v>5.8220000000000001</v>
       </c>
       <c r="G39">
-        <v>6.9089999999999998</v>
+        <v>6.7069999999999999</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -6033,7 +6030,7 @@
         <v>6.7119999999999997</v>
       </c>
       <c r="G40">
-        <v>7.54</v>
+        <v>7.4509999999999996</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -6053,7 +6050,7 @@
         <v>7.7889999999999997</v>
       </c>
       <c r="G41">
-        <v>8.2479999999999993</v>
+        <v>8.266</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -6073,7 +6070,7 @@
         <v>9.0039999999999996</v>
       </c>
       <c r="G42">
-        <v>9.0210000000000008</v>
+        <v>9.1129999999999995</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -6083,9 +6080,6 @@
       <c r="C43">
         <v>9.0830000000000002</v>
       </c>
-      <c r="G43">
-        <v>9.8529999999999998</v>
-      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
@@ -6093,221 +6087,6 @@
       </c>
       <c r="C44">
         <v>9.6159999999999997</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G45">
-        <v>11.65</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G46">
-        <v>12.65</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G47">
-        <v>13.7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G48">
-        <v>14.82</v>
-      </c>
-    </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G49">
-        <v>16.010000000000002</v>
-      </c>
-    </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G50">
-        <v>17.32</v>
-      </c>
-    </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G51">
-        <v>18.72</v>
-      </c>
-    </row>
-    <row r="52" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G52">
-        <v>20.260000000000002</v>
-      </c>
-    </row>
-    <row r="53" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G53">
-        <v>21.95</v>
-      </c>
-    </row>
-    <row r="54" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G54">
-        <v>23.79</v>
-      </c>
-    </row>
-    <row r="55" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G55">
-        <v>25.73</v>
-      </c>
-    </row>
-    <row r="56" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G56">
-        <v>27.85</v>
-      </c>
-    </row>
-    <row r="57" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G57">
-        <v>30.18</v>
-      </c>
-    </row>
-    <row r="58" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G58">
-        <v>32.65</v>
-      </c>
-    </row>
-    <row r="59" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G59">
-        <v>35.380000000000003</v>
-      </c>
-    </row>
-    <row r="60" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G60">
-        <v>38.299999999999997</v>
-      </c>
-    </row>
-    <row r="61" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G61">
-        <v>41.43</v>
-      </c>
-    </row>
-    <row r="62" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G62">
-        <v>44.83</v>
-      </c>
-    </row>
-    <row r="63" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G63">
-        <v>48.56</v>
-      </c>
-    </row>
-    <row r="64" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G64">
-        <v>52.79</v>
-      </c>
-    </row>
-    <row r="65" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G65">
-        <v>57.37</v>
-      </c>
-    </row>
-    <row r="66" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G66">
-        <v>62.44</v>
-      </c>
-    </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G67">
-        <v>67.94</v>
-      </c>
-    </row>
-    <row r="68" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G68">
-        <v>74.11</v>
-      </c>
-    </row>
-    <row r="69" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G69">
-        <v>80.98</v>
-      </c>
-    </row>
-    <row r="70" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G70">
-        <v>88.7</v>
-      </c>
-    </row>
-    <row r="71" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G71">
-        <v>97.29</v>
-      </c>
-    </row>
-    <row r="72" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G72">
-        <v>107.3</v>
-      </c>
-    </row>
-    <row r="73" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G73">
-        <v>118.3</v>
-      </c>
-    </row>
-    <row r="74" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G74">
-        <v>130.5</v>
-      </c>
-    </row>
-    <row r="75" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G75">
-        <v>144.4</v>
-      </c>
-    </row>
-    <row r="76" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G76">
-        <v>159.9</v>
-      </c>
-    </row>
-    <row r="77" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G77">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="78" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G78">
-        <v>199.2</v>
-      </c>
-    </row>
-    <row r="79" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G79">
-        <v>224.9</v>
-      </c>
-    </row>
-    <row r="80" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G80">
-        <v>254.4</v>
-      </c>
-    </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G81">
-        <v>290.2</v>
-      </c>
-    </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G82">
-        <v>334.4</v>
-      </c>
-    </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G83">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G84">
-        <v>456.7</v>
-      </c>
-    </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G85">
-        <v>545.5</v>
-      </c>
-    </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G86">
-        <v>667.6</v>
-      </c>
-    </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G87">
-        <v>865.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for sens vs. error Excel plot for devreseek [5f8fbc4]
</commit_message>
<xml_diff>
--- a/results/sensitivity_vs_error.xlsx
+++ b/results/sensitivity_vs_error.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\reseek_scop40\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A5F507-50F5-4079-8D73-97F1FC9E3854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A896C3D1-E1C4-4A40-99D4-C59C56DBAEF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{30A151E1-5A68-4C81-B266-04173DADF783}"/>
+    <workbookView xWindow="2070" yWindow="4335" windowWidth="23940" windowHeight="15420" xr2:uid="{30A151E1-5A68-4C81-B266-04173DADF783}"/>
   </bookViews>
   <sheets>
     <sheet name="SF" sheetId="9" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>fpepq</t>
   </si>
@@ -57,7 +57,10 @@
     <t>Reseek</t>
   </si>
   <si>
-    <t>GTalign</t>
+    <t>devreseek-sensitive</t>
+  </si>
+  <si>
+    <t>Reseek-sensitive</t>
   </si>
 </sst>
 </file>
@@ -988,162 +991,8 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="5"/>
+          <c:idx val="2"/>
           <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>SF!$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>GTalign</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:prstDash val="sysDot"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>SF!$G$2:$G$44</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="43"/>
-                <c:pt idx="5">
-                  <c:v>1.5339999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.266E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.3000000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.6829999999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6.1190000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>8.1079999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.1046</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.12870000000000001</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.15790000000000001</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.1946</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.23680000000000001</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.28460000000000002</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.34079999999999999</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.40810000000000002</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.4899</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.57689999999999997</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.68110000000000004</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.81289999999999996</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.95940000000000003</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1.1279999999999999</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1.3340000000000001</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1.548</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1.7929999999999999</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2.08</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2.4009999999999998</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2.7679999999999998</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>3.1880000000000002</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>3.6619999999999999</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>4.1689999999999996</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>4.7380000000000004</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>5.3369999999999997</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>5.9909999999999997</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>6.7069999999999999</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>7.4509999999999996</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>8.266</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>9.1129999999999995</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F309-4D48-AF9D-5CD1365FCBDA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>SF!$D$1</c:f>
@@ -1435,7 +1284,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="5"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>SF!$F$1</c:f>
@@ -1604,100 +1453,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="44"/>
                 <c:pt idx="9">
-                  <c:v>1.472E-2</c:v>
+                  <c:v>1.418E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.3910000000000001E-2</c:v>
+                  <c:v>2.2919999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.202E-2</c:v>
+                  <c:v>3.4250000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.5400000000000003E-2</c:v>
+                  <c:v>4.8520000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.0650000000000003E-2</c:v>
+                  <c:v>6.5379999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.9920000000000005E-2</c:v>
+                  <c:v>8.5089999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.1031</c:v>
+                  <c:v>0.11310000000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.1308</c:v>
+                  <c:v>0.1457</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.1646</c:v>
+                  <c:v>0.17899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.20680000000000001</c:v>
+                  <c:v>0.22489999999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.26140000000000002</c:v>
+                  <c:v>0.28120000000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.31859999999999999</c:v>
+                  <c:v>0.34720000000000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.38900000000000001</c:v>
+                  <c:v>0.42899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.47089999999999999</c:v>
+                  <c:v>0.52859999999999996</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.56610000000000005</c:v>
+                  <c:v>0.6462</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.68659999999999999</c:v>
+                  <c:v>0.79359999999999997</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.83130000000000004</c:v>
+                  <c:v>0.96650000000000003</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.002</c:v>
+                  <c:v>1.18</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.204</c:v>
+                  <c:v>1.4330000000000001</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.4319999999999999</c:v>
+                  <c:v>1.742</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.704</c:v>
+                  <c:v>2.1269999999999998</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.0009999999999999</c:v>
+                  <c:v>2.6160000000000001</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.34</c:v>
+                  <c:v>3.2490000000000001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.7370000000000001</c:v>
+                  <c:v>4.1619999999999999</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.1989999999999998</c:v>
+                  <c:v>5.5209999999999999</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.7120000000000002</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>4.3129999999999997</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>5.0250000000000004</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>5.8220000000000001</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>6.7119999999999997</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>7.7889999999999997</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>9.0039999999999996</c:v>
+                  <c:v>8.0180000000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1706,6 +1537,147 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-BEEB-47F3-8EDD-6D5CB1B06A4F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SF!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Reseek-sensitive</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="50800" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>SF!$G$2:$G$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="9">
+                  <c:v>1.418E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.248E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.2559999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.7539999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.4579999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.5269999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.1119</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.1474</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.1918</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.24129999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.30509999999999998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.3846</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.4824</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.59799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.73080000000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.88729999999999998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.0649999999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.4990000000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.7669999999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.073</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.407</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.762</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.2360000000000002</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.6869999999999998</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.2089999999999996</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.8659999999999997</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.5049999999999999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6.2610000000000001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7.157</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8.0990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>9.2430000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F309-4D48-AF9D-5CD1365FCBDA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2910,165 +2882,8 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="5"/>
+          <c:idx val="3"/>
           <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Fold!$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>GTalign</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:prstDash val="sysDot"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Fold!$G$2:$G$44</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="43"/>
-                <c:pt idx="5">
-                  <c:v>1.516E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.614E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.916E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6.0569999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>8.7410000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.1202</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.16489999999999999</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.21029999999999999</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.2671</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.33400000000000002</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.41920000000000002</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.51439999999999997</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.61539999999999995</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.7379</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.88560000000000005</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.038</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.2130000000000001</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.403</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1.599</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1.821</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2.0529999999999999</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2.2989999999999999</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2.581</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2.8889999999999998</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>3.218</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>3.556</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>3.9249999999999998</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>4.3259999999999996</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>4.7690000000000001</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>5.24</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>5.7439999999999998</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>6.3239999999999998</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>6.9089999999999998</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>7.54</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>8.2479999999999993</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>9.0210000000000008</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>9.8529999999999998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-16FC-45E1-AA5C-364965FBEF56}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>Fold!$E$1</c:f>
@@ -3326,7 +3141,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="5"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>Fold!$F$1</c:f>
@@ -3495,68 +3310,50 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="44"/>
+                <c:pt idx="5">
+                  <c:v>1.1950000000000001E-2</c:v>
+                </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.5339999999999999E-2</c:v>
+                  <c:v>2.069E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.3990000000000001E-2</c:v>
+                  <c:v>3.175E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.6749999999999998E-2</c:v>
+                  <c:v>5.058E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.7090000000000002E-2</c:v>
+                  <c:v>7.9740000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.6699999999999999E-2</c:v>
+                  <c:v>0.1229</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.13009999999999999</c:v>
+                  <c:v>0.2031</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.19450000000000001</c:v>
+                  <c:v>0.32400000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.2843</c:v>
+                  <c:v>0.50919999999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.41510000000000002</c:v>
+                  <c:v>0.78349999999999997</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.57630000000000003</c:v>
+                  <c:v>1.1950000000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.79010000000000002</c:v>
+                  <c:v>1.8320000000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.0589999999999999</c:v>
+                  <c:v>2.911</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.3919999999999999</c:v>
+                  <c:v>5.0650000000000004</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.7989999999999999</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2.2759999999999998</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2.8530000000000002</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>3.5590000000000002</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>4.43</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>5.4809999999999999</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>6.7619999999999996</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>8.3040000000000003</c:v>
+                  <c:v>22.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3565,6 +3362,165 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-7427-4367-9DFB-FBF38ECB406C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Fold!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>devreseek-sensitive</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="50800" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Fold!$G$2:$G$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="5">
+                  <c:v>1.044E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7659999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.7650000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.0320000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.164E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.5170000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.1409</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.20050000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.2903</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.41060000000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.57069999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.76549999999999996</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.004</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.2849999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.643</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.097</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.6379999999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.2290000000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.9580000000000002</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.8739999999999997</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.8250000000000002</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7.1609999999999996</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8.6920000000000002</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10.39</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>12.63</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>14.92</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>18.25</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>22.1</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>26.81</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>32.94</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>40.25</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>50.01</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>62.46</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>79.41</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>101.9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>179.5</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>251.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-16FC-45E1-AA5C-364965FBEF56}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5024,16 +4980,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>200026</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>123826</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:rowOff>114299</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>238126</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>161926</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5425,14 +5381,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D48A558-673B-4B1E-8FF7-FCB07FA6F0FA}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
     <col min="14" max="14" width="13.7109375" customWidth="1"/>
     <col min="15" max="15" width="15.140625" customWidth="1"/>
   </cols>
@@ -5457,7 +5412,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -5507,9 +5462,6 @@
       <c r="E7">
         <v>1.222E-2</v>
       </c>
-      <c r="G7">
-        <v>1.5339999999999999E-2</v>
-      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -5524,9 +5476,6 @@
       <c r="E8">
         <v>2.3640000000000001E-2</v>
       </c>
-      <c r="G8">
-        <v>2.266E-2</v>
-      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -5544,9 +5493,6 @@
       <c r="E9">
         <v>3.9600000000000003E-2</v>
       </c>
-      <c r="G9">
-        <v>3.3000000000000002E-2</v>
-      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -5564,9 +5510,6 @@
       <c r="E10">
         <v>6.012E-2</v>
       </c>
-      <c r="G10">
-        <v>4.6829999999999997E-2</v>
-      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -5585,10 +5528,10 @@
         <v>8.5900000000000004E-2</v>
       </c>
       <c r="F11">
-        <v>1.472E-2</v>
+        <v>1.418E-2</v>
       </c>
       <c r="G11">
-        <v>6.1190000000000001E-2</v>
+        <v>1.418E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -5608,10 +5551,10 @@
         <v>0.11609999999999999</v>
       </c>
       <c r="F12">
-        <v>2.3910000000000001E-2</v>
+        <v>2.2919999999999999E-2</v>
       </c>
       <c r="G12">
-        <v>8.1079999999999999E-2</v>
+        <v>2.248E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -5631,10 +5574,10 @@
         <v>0.15129999999999999</v>
       </c>
       <c r="F13">
-        <v>3.202E-2</v>
+        <v>3.4250000000000003E-2</v>
       </c>
       <c r="G13">
-        <v>0.1046</v>
+        <v>3.2559999999999999E-2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -5651,10 +5594,10 @@
         <v>0.19400000000000001</v>
       </c>
       <c r="F14">
-        <v>4.5400000000000003E-2</v>
+        <v>4.8520000000000001E-2</v>
       </c>
       <c r="G14">
-        <v>0.12870000000000001</v>
+        <v>4.7539999999999999E-2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -5671,10 +5614,10 @@
         <v>0.2422</v>
       </c>
       <c r="F15">
-        <v>6.0650000000000003E-2</v>
+        <v>6.5379999999999994E-2</v>
       </c>
       <c r="G15">
-        <v>0.15790000000000001</v>
+        <v>6.4579999999999999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -5691,10 +5634,10 @@
         <v>0.29699999999999999</v>
       </c>
       <c r="F16">
-        <v>7.9920000000000005E-2</v>
+        <v>8.5089999999999999E-2</v>
       </c>
       <c r="G16">
-        <v>0.1946</v>
+        <v>8.5269999999999999E-2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -5711,10 +5654,10 @@
         <v>0.36520000000000002</v>
       </c>
       <c r="F17">
-        <v>0.1031</v>
+        <v>0.11310000000000001</v>
       </c>
       <c r="G17">
-        <v>0.23680000000000001</v>
+        <v>0.1119</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -5731,10 +5674,10 @@
         <v>0.43440000000000001</v>
       </c>
       <c r="F18">
-        <v>0.1308</v>
+        <v>0.1457</v>
       </c>
       <c r="G18">
-        <v>0.28460000000000002</v>
+        <v>0.1474</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -5751,10 +5694,10 @@
         <v>0.5151</v>
       </c>
       <c r="F19">
-        <v>0.1646</v>
+        <v>0.17899999999999999</v>
       </c>
       <c r="G19">
-        <v>0.34079999999999999</v>
+        <v>0.1918</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -5771,10 +5714,10 @@
         <v>0.60899999999999999</v>
       </c>
       <c r="F20">
-        <v>0.20680000000000001</v>
+        <v>0.22489999999999999</v>
       </c>
       <c r="G20">
-        <v>0.40810000000000002</v>
+        <v>0.24129999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -5791,10 +5734,10 @@
         <v>0.70930000000000004</v>
       </c>
       <c r="F21">
-        <v>0.26140000000000002</v>
+        <v>0.28120000000000001</v>
       </c>
       <c r="G21">
-        <v>0.4899</v>
+        <v>0.30509999999999998</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -5811,10 +5754,10 @@
         <v>0.82320000000000004</v>
       </c>
       <c r="F22">
-        <v>0.31859999999999999</v>
+        <v>0.34720000000000001</v>
       </c>
       <c r="G22">
-        <v>0.57689999999999997</v>
+        <v>0.3846</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -5831,10 +5774,10 @@
         <v>0.94620000000000004</v>
       </c>
       <c r="F23">
-        <v>0.38900000000000001</v>
+        <v>0.42899999999999999</v>
       </c>
       <c r="G23">
-        <v>0.68110000000000004</v>
+        <v>0.4824</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -5851,10 +5794,10 @@
         <v>1.08</v>
       </c>
       <c r="F24">
-        <v>0.47089999999999999</v>
+        <v>0.52859999999999996</v>
       </c>
       <c r="G24">
-        <v>0.81289999999999996</v>
+        <v>0.59799999999999998</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -5871,10 +5814,10 @@
         <v>1.238</v>
       </c>
       <c r="F25">
-        <v>0.56610000000000005</v>
+        <v>0.6462</v>
       </c>
       <c r="G25">
-        <v>0.95940000000000003</v>
+        <v>0.73080000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -5891,10 +5834,10 @@
         <v>1.4179999999999999</v>
       </c>
       <c r="F26">
-        <v>0.68659999999999999</v>
+        <v>0.79359999999999997</v>
       </c>
       <c r="G26">
-        <v>1.1279999999999999</v>
+        <v>0.88729999999999998</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -5911,10 +5854,10 @@
         <v>1.617</v>
       </c>
       <c r="F27">
-        <v>0.83130000000000004</v>
+        <v>0.96650000000000003</v>
       </c>
       <c r="G27">
-        <v>1.3340000000000001</v>
+        <v>1.0649999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -5931,10 +5874,10 @@
         <v>1.83</v>
       </c>
       <c r="F28">
-        <v>1.002</v>
+        <v>1.18</v>
       </c>
       <c r="G28">
-        <v>1.548</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -5951,10 +5894,10 @@
         <v>2.0739999999999998</v>
       </c>
       <c r="F29">
-        <v>1.204</v>
+        <v>1.4330000000000001</v>
       </c>
       <c r="G29">
-        <v>1.7929999999999999</v>
+        <v>1.4990000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -5971,10 +5914,10 @@
         <v>2.3559999999999999</v>
       </c>
       <c r="F30">
-        <v>1.4319999999999999</v>
+        <v>1.742</v>
       </c>
       <c r="G30">
-        <v>2.08</v>
+        <v>1.7669999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -5991,10 +5934,10 @@
         <v>2.6779999999999999</v>
       </c>
       <c r="F31">
-        <v>1.704</v>
+        <v>2.1269999999999998</v>
       </c>
       <c r="G31">
-        <v>2.4009999999999998</v>
+        <v>2.073</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -6011,10 +5954,10 @@
         <v>3.036</v>
       </c>
       <c r="F32">
-        <v>2.0009999999999999</v>
+        <v>2.6160000000000001</v>
       </c>
       <c r="G32">
-        <v>2.7679999999999998</v>
+        <v>2.407</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -6031,10 +5974,10 @@
         <v>3.4319999999999999</v>
       </c>
       <c r="F33">
-        <v>2.34</v>
+        <v>3.2490000000000001</v>
       </c>
       <c r="G33">
-        <v>3.1880000000000002</v>
+        <v>2.762</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -6051,10 +5994,10 @@
         <v>3.8820000000000001</v>
       </c>
       <c r="F34">
-        <v>2.7370000000000001</v>
+        <v>4.1619999999999999</v>
       </c>
       <c r="G34">
-        <v>3.6619999999999999</v>
+        <v>3.2360000000000002</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -6071,10 +6014,10 @@
         <v>4.3789999999999996</v>
       </c>
       <c r="F35">
-        <v>3.1989999999999998</v>
+        <v>5.5209999999999999</v>
       </c>
       <c r="G35">
-        <v>4.1689999999999996</v>
+        <v>3.6869999999999998</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -6091,10 +6034,10 @@
         <v>4.9329999999999998</v>
       </c>
       <c r="F36">
-        <v>3.7120000000000002</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="G36">
-        <v>4.7380000000000004</v>
+        <v>4.2089999999999996</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -6110,11 +6053,8 @@
       <c r="E37">
         <v>5.5570000000000004</v>
       </c>
-      <c r="F37">
-        <v>4.3129999999999997</v>
-      </c>
       <c r="G37">
-        <v>5.3369999999999997</v>
+        <v>4.8659999999999997</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -6130,11 +6070,8 @@
       <c r="E38">
         <v>6.2430000000000003</v>
       </c>
-      <c r="F38">
-        <v>5.0250000000000004</v>
-      </c>
       <c r="G38">
-        <v>5.9909999999999997</v>
+        <v>5.5049999999999999</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -6150,11 +6087,8 @@
       <c r="E39">
         <v>7.0279999999999996</v>
       </c>
-      <c r="F39">
-        <v>5.8220000000000001</v>
-      </c>
       <c r="G39">
-        <v>6.7069999999999999</v>
+        <v>6.2610000000000001</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -6170,11 +6104,8 @@
       <c r="E40">
         <v>7.9009999999999998</v>
       </c>
-      <c r="F40">
-        <v>6.7119999999999997</v>
-      </c>
       <c r="G40">
-        <v>7.4509999999999996</v>
+        <v>7.157</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -6190,11 +6121,8 @@
       <c r="E41">
         <v>8.85</v>
       </c>
-      <c r="F41">
-        <v>7.7889999999999997</v>
-      </c>
       <c r="G41">
-        <v>8.266</v>
+        <v>8.0990000000000002</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -6210,11 +6138,8 @@
       <c r="E42">
         <v>9.9809999999999999</v>
       </c>
-      <c r="F42">
-        <v>9.0039999999999996</v>
-      </c>
       <c r="G42">
-        <v>9.1129999999999995</v>
+        <v>9.2430000000000003</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -6241,17 +6166,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD5C0124-FDAB-4252-836F-9CFDB475E886}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S31" sqref="S31"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -6339,8 +6263,11 @@
       <c r="E7">
         <v>5.985E-2</v>
       </c>
+      <c r="F7">
+        <v>1.1950000000000001E-2</v>
+      </c>
       <c r="G7">
-        <v>1.516E-2</v>
+        <v>1.044E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -6357,10 +6284,10 @@
         <v>7.7600000000000002E-2</v>
       </c>
       <c r="F8">
-        <v>1.5339999999999999E-2</v>
+        <v>2.069E-2</v>
       </c>
       <c r="G8">
-        <v>2.614E-2</v>
+        <v>1.7659999999999999E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -6377,10 +6304,10 @@
         <v>9.8390000000000005E-2</v>
       </c>
       <c r="F9">
-        <v>2.3990000000000001E-2</v>
+        <v>3.175E-2</v>
       </c>
       <c r="G9">
-        <v>3.916E-2</v>
+        <v>2.7650000000000001E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -6397,10 +6324,10 @@
         <v>0.122</v>
       </c>
       <c r="F10">
-        <v>3.6749999999999998E-2</v>
+        <v>5.058E-2</v>
       </c>
       <c r="G10">
-        <v>6.0569999999999999E-2</v>
+        <v>4.0320000000000002E-2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -6417,10 +6344,10 @@
         <v>0.15409999999999999</v>
       </c>
       <c r="F11">
-        <v>5.7090000000000002E-2</v>
+        <v>7.9740000000000005E-2</v>
       </c>
       <c r="G11">
-        <v>8.7410000000000002E-2</v>
+        <v>6.164E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -6437,10 +6364,10 @@
         <v>0.1905</v>
       </c>
       <c r="F12">
-        <v>8.6699999999999999E-2</v>
+        <v>0.1229</v>
       </c>
       <c r="G12">
-        <v>0.1202</v>
+        <v>9.5170000000000005E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -6457,10 +6384,10 @@
         <v>0.2407</v>
       </c>
       <c r="F13">
-        <v>0.13009999999999999</v>
+        <v>0.2031</v>
       </c>
       <c r="G13">
-        <v>0.16489999999999999</v>
+        <v>0.1409</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -6477,10 +6404,10 @@
         <v>0.30919999999999997</v>
       </c>
       <c r="F14">
-        <v>0.19450000000000001</v>
+        <v>0.32400000000000001</v>
       </c>
       <c r="G14">
-        <v>0.21029999999999999</v>
+        <v>0.20050000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -6497,10 +6424,10 @@
         <v>0.39729999999999999</v>
       </c>
       <c r="F15">
-        <v>0.2843</v>
+        <v>0.50919999999999999</v>
       </c>
       <c r="G15">
-        <v>0.2671</v>
+        <v>0.2903</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -6517,10 +6444,10 @@
         <v>0.5242</v>
       </c>
       <c r="F16">
-        <v>0.41510000000000002</v>
+        <v>0.78349999999999997</v>
       </c>
       <c r="G16">
-        <v>0.33400000000000002</v>
+        <v>0.41060000000000002</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -6537,10 +6464,10 @@
         <v>0.68600000000000005</v>
       </c>
       <c r="F17">
-        <v>0.57630000000000003</v>
+        <v>1.1950000000000001</v>
       </c>
       <c r="G17">
-        <v>0.41920000000000002</v>
+        <v>0.57069999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -6557,10 +6484,10 @@
         <v>0.8881</v>
       </c>
       <c r="F18">
-        <v>0.79010000000000002</v>
+        <v>1.8320000000000001</v>
       </c>
       <c r="G18">
-        <v>0.51439999999999997</v>
+        <v>0.76549999999999996</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -6577,10 +6504,10 @@
         <v>1.147</v>
       </c>
       <c r="F19">
-        <v>1.0589999999999999</v>
+        <v>2.911</v>
       </c>
       <c r="G19">
-        <v>0.61539999999999995</v>
+        <v>1.004</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -6597,10 +6524,10 @@
         <v>1.46</v>
       </c>
       <c r="F20">
-        <v>1.3919999999999999</v>
+        <v>5.0650000000000004</v>
       </c>
       <c r="G20">
-        <v>0.7379</v>
+        <v>1.2849999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -6617,10 +6544,10 @@
         <v>1.841</v>
       </c>
       <c r="F21">
-        <v>1.7989999999999999</v>
+        <v>22.65</v>
       </c>
       <c r="G21">
-        <v>0.88560000000000005</v>
+        <v>1.643</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -6636,11 +6563,8 @@
       <c r="E22">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F22">
-        <v>2.2759999999999998</v>
-      </c>
       <c r="G22">
-        <v>1.038</v>
+        <v>2.097</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -6656,11 +6580,8 @@
       <c r="E23">
         <v>2.819</v>
       </c>
-      <c r="F23">
-        <v>2.8530000000000002</v>
-      </c>
       <c r="G23">
-        <v>1.2130000000000001</v>
+        <v>2.6379999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -6676,11 +6597,8 @@
       <c r="E24">
         <v>3.4220000000000002</v>
       </c>
-      <c r="F24">
-        <v>3.5590000000000002</v>
-      </c>
       <c r="G24">
-        <v>1.403</v>
+        <v>3.2290000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -6696,11 +6614,8 @@
       <c r="E25">
         <v>4.1360000000000001</v>
       </c>
-      <c r="F25">
-        <v>4.43</v>
-      </c>
       <c r="G25">
-        <v>1.599</v>
+        <v>3.9580000000000002</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -6716,11 +6631,8 @@
       <c r="E26">
         <v>4.944</v>
       </c>
-      <c r="F26">
-        <v>5.4809999999999999</v>
-      </c>
       <c r="G26">
-        <v>1.821</v>
+        <v>4.8739999999999997</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -6736,11 +6648,8 @@
       <c r="E27">
         <v>5.8440000000000003</v>
       </c>
-      <c r="F27">
-        <v>6.7619999999999996</v>
-      </c>
       <c r="G27">
-        <v>2.0529999999999999</v>
+        <v>5.8250000000000002</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -6756,11 +6665,8 @@
       <c r="E28">
         <v>6.8609999999999998</v>
       </c>
-      <c r="F28">
-        <v>8.3040000000000003</v>
-      </c>
       <c r="G28">
-        <v>2.2989999999999999</v>
+        <v>7.1609999999999996</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -6777,7 +6683,7 @@
         <v>7.9749999999999996</v>
       </c>
       <c r="G29">
-        <v>2.581</v>
+        <v>8.6920000000000002</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -6794,7 +6700,7 @@
         <v>9.1880000000000006</v>
       </c>
       <c r="G30">
-        <v>2.8889999999999998</v>
+        <v>10.39</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -6808,7 +6714,7 @@
         <v>2.9729999999999999</v>
       </c>
       <c r="G31">
-        <v>3.218</v>
+        <v>12.63</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -6822,7 +6728,7 @@
         <v>3.3010000000000002</v>
       </c>
       <c r="G32">
-        <v>3.556</v>
+        <v>14.92</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -6836,7 +6742,7 @@
         <v>3.6440000000000001</v>
       </c>
       <c r="G33">
-        <v>3.9249999999999998</v>
+        <v>18.25</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -6850,7 +6756,7 @@
         <v>4.0289999999999999</v>
       </c>
       <c r="G34">
-        <v>4.3259999999999996</v>
+        <v>22.1</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -6864,7 +6770,7 @@
         <v>4.4219999999999997</v>
       </c>
       <c r="G35">
-        <v>4.7690000000000001</v>
+        <v>26.81</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -6878,7 +6784,7 @@
         <v>4.8380000000000001</v>
       </c>
       <c r="G36">
-        <v>5.24</v>
+        <v>32.94</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -6892,7 +6798,7 @@
         <v>5.2830000000000004</v>
       </c>
       <c r="G37">
-        <v>5.7439999999999998</v>
+        <v>40.25</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -6903,7 +6809,7 @@
         <v>5.7839999999999998</v>
       </c>
       <c r="G38">
-        <v>6.3239999999999998</v>
+        <v>50.01</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -6914,7 +6820,7 @@
         <v>6.3049999999999997</v>
       </c>
       <c r="G39">
-        <v>6.9089999999999998</v>
+        <v>62.46</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -6925,7 +6831,7 @@
         <v>6.8719999999999999</v>
       </c>
       <c r="G40">
-        <v>7.54</v>
+        <v>79.41</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -6936,7 +6842,7 @@
         <v>7.49</v>
       </c>
       <c r="G41">
-        <v>8.2479999999999993</v>
+        <v>101.9</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -6947,7 +6853,7 @@
         <v>8.1359999999999992</v>
       </c>
       <c r="G42">
-        <v>9.0210000000000008</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -6958,7 +6864,7 @@
         <v>8.8119999999999994</v>
       </c>
       <c r="G43">
-        <v>9.8529999999999998</v>
+        <v>179.5</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -6967,6 +6873,14 @@
       </c>
       <c r="D44">
         <v>9.5589999999999993</v>
+      </c>
+      <c r="G44">
+        <v>251.3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G45">
+        <v>603.79999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for reseek [7e7be2b]
</commit_message>
<xml_diff>
--- a/results/sensitivity_vs_error.xlsx
+++ b/results/sensitivity_vs_error.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\reseek_scop40\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A896C3D1-E1C4-4A40-99D4-C59C56DBAEF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E878C3BF-C421-4054-980D-8689E9C81298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="4335" windowWidth="23940" windowHeight="15420" xr2:uid="{30A151E1-5A68-4C81-B266-04173DADF783}"/>
+    <workbookView xWindow="2070" yWindow="4335" windowWidth="23940" windowHeight="15420" activeTab="1" xr2:uid="{30A151E1-5A68-4C81-B266-04173DADF783}"/>
   </bookViews>
   <sheets>
     <sheet name="SF" sheetId="9" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>fpepq</t>
   </si>
@@ -60,7 +60,10 @@
     <t>devreseek-sensitive</t>
   </si>
   <si>
-    <t>Reseek-sensitive</t>
+    <t>devreseek</t>
+  </si>
+  <si>
+    <t>Reseek-sens</t>
   </si>
 </sst>
 </file>
@@ -1453,82 +1456,88 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="44"/>
                 <c:pt idx="9">
-                  <c:v>1.418E-2</c:v>
+                  <c:v>1.204E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.2919999999999999E-2</c:v>
+                  <c:v>1.9449999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.4250000000000003E-2</c:v>
+                  <c:v>3.006E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.8520000000000001E-2</c:v>
+                  <c:v>4.2819999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.5379999999999994E-2</c:v>
+                  <c:v>5.7709999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8.5089999999999999E-2</c:v>
+                  <c:v>7.6439999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.11310000000000001</c:v>
+                  <c:v>0.10199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.1457</c:v>
+                  <c:v>0.13289999999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.17899999999999999</c:v>
+                  <c:v>0.1643</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.22489999999999999</c:v>
+                  <c:v>0.20669999999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.28120000000000001</c:v>
+                  <c:v>0.25790000000000002</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.34720000000000001</c:v>
+                  <c:v>0.31940000000000002</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.42899999999999999</c:v>
+                  <c:v>0.39550000000000002</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.52859999999999996</c:v>
+                  <c:v>0.49099999999999999</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.6462</c:v>
+                  <c:v>0.60060000000000002</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.79359999999999997</c:v>
+                  <c:v>0.74009999999999998</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.96650000000000003</c:v>
+                  <c:v>0.90049999999999997</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.18</c:v>
+                  <c:v>1.095</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.4330000000000001</c:v>
+                  <c:v>1.33</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.742</c:v>
+                  <c:v>1.6080000000000001</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.1269999999999998</c:v>
+                  <c:v>1.954</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.6160000000000001</c:v>
+                  <c:v>2.3690000000000002</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.2490000000000001</c:v>
+                  <c:v>2.8860000000000001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.1619999999999999</c:v>
+                  <c:v>3.544</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>5.5209999999999999</c:v>
+                  <c:v>4.3579999999999997</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8.0180000000000007</c:v>
+                  <c:v>5.3819999999999997</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6.9409999999999998</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9.1479999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1549,7 +1558,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Reseek-sensitive</c:v>
+                  <c:v>Reseek-sens</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1576,100 +1585,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="43"/>
                 <c:pt idx="9">
-                  <c:v>1.418E-2</c:v>
+                  <c:v>1.1679999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.248E-2</c:v>
+                  <c:v>1.882E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.2559999999999999E-2</c:v>
+                  <c:v>2.819E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.7539999999999999E-2</c:v>
+                  <c:v>4.1300000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.4579999999999999E-2</c:v>
+                  <c:v>5.7270000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8.5269999999999999E-2</c:v>
+                  <c:v>7.671E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.1119</c:v>
+                  <c:v>0.10349999999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.1474</c:v>
+                  <c:v>0.1366</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.1918</c:v>
+                  <c:v>0.1804</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.24129999999999999</c:v>
+                  <c:v>0.22650000000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.30509999999999998</c:v>
+                  <c:v>0.28560000000000002</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.3846</c:v>
+                  <c:v>0.36120000000000002</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.4824</c:v>
+                  <c:v>0.45379999999999998</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.59799999999999998</c:v>
+                  <c:v>0.56469999999999998</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.73080000000000001</c:v>
+                  <c:v>0.69489999999999996</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.88729999999999998</c:v>
+                  <c:v>0.8458</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.0649999999999999</c:v>
+                  <c:v>1.018</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.26</c:v>
+                  <c:v>1.21</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.4990000000000001</c:v>
+                  <c:v>1.45</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.7669999999999999</c:v>
+                  <c:v>1.7170000000000001</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.073</c:v>
+                  <c:v>2.0179999999999998</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.407</c:v>
+                  <c:v>2.355</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.762</c:v>
+                  <c:v>2.7170000000000001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.2360000000000002</c:v>
+                  <c:v>3.1949999999999998</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.6869999999999998</c:v>
+                  <c:v>3.6389999999999998</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4.2089999999999996</c:v>
+                  <c:v>4.1580000000000004</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.8659999999999997</c:v>
+                  <c:v>4.7910000000000004</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>5.5049999999999999</c:v>
+                  <c:v>5.431</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>6.2610000000000001</c:v>
+                  <c:v>6.2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>7.157</c:v>
+                  <c:v>7.0449999999999999</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>8.0990000000000002</c:v>
+                  <c:v>7.9409999999999998</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>9.2430000000000003</c:v>
+                  <c:v>9.0619999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3148,7 +3157,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Reseek</c:v>
+                  <c:v>devreseek</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3310,50 +3319,56 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="44"/>
-                <c:pt idx="5">
-                  <c:v>1.1950000000000001E-2</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.069E-2</c:v>
+                  <c:v>1.204E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.175E-2</c:v>
+                  <c:v>1.9449999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.058E-2</c:v>
+                  <c:v>3.4520000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.9740000000000005E-2</c:v>
+                  <c:v>6.1100000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1229</c:v>
+                  <c:v>0.1038</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.2031</c:v>
+                  <c:v>0.186</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.32400000000000001</c:v>
+                  <c:v>0.31140000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.50919999999999999</c:v>
+                  <c:v>0.4768</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.78349999999999997</c:v>
+                  <c:v>0.73850000000000005</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.1950000000000001</c:v>
+                  <c:v>1.0840000000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.8320000000000001</c:v>
+                  <c:v>1.5720000000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.911</c:v>
+                  <c:v>2.294</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.0650000000000004</c:v>
+                  <c:v>3.2949999999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>22.65</c:v>
+                  <c:v>4.8680000000000003</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.5640000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>13.13</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>56.99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3400,119 +3415,113 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="43"/>
-                <c:pt idx="5">
-                  <c:v>1.044E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.7659999999999999E-2</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.7650000000000001E-2</c:v>
+                  <c:v>1.686E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.0320000000000002E-2</c:v>
+                  <c:v>2.605E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.164E-2</c:v>
+                  <c:v>4.326E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.5170000000000005E-2</c:v>
+                  <c:v>7.3230000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.1409</c:v>
+                  <c:v>0.1168</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.20050000000000001</c:v>
+                  <c:v>0.1754</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.2903</c:v>
+                  <c:v>0.26600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.41060000000000002</c:v>
+                  <c:v>0.38579999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.57069999999999999</c:v>
+                  <c:v>0.54569999999999996</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.76549999999999996</c:v>
+                  <c:v>0.74450000000000005</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.004</c:v>
+                  <c:v>0.98280000000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.2849999999999999</c:v>
+                  <c:v>1.2669999999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.643</c:v>
+                  <c:v>1.625</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.097</c:v>
+                  <c:v>2.08</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.6379999999999999</c:v>
+                  <c:v>2.61</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.2290000000000001</c:v>
+                  <c:v>3.165</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.9580000000000002</c:v>
+                  <c:v>3.9</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4.8739999999999997</c:v>
+                  <c:v>4.7370000000000001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5.8250000000000002</c:v>
+                  <c:v>5.6870000000000003</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.1609999999999996</c:v>
+                  <c:v>6.9249999999999998</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>8.6920000000000002</c:v>
+                  <c:v>8.1839999999999993</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>10.39</c:v>
+                  <c:v>9.8940000000000001</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>12.63</c:v>
+                  <c:v>11.57</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>14.92</c:v>
+                  <c:v>13.95</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>18.25</c:v>
+                  <c:v>16.43</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>22.1</c:v>
+                  <c:v>19.670000000000002</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>26.81</c:v>
+                  <c:v>23.36</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>32.94</c:v>
+                  <c:v>27.85</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>40.25</c:v>
+                  <c:v>33.39</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>50.01</c:v>
+                  <c:v>39.96</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>62.46</c:v>
+                  <c:v>48.32</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>79.41</c:v>
+                  <c:v>58.22</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>101.9</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>133</c:v>
+                  <c:v>87.23</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>179.5</c:v>
+                  <c:v>108.7</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>251.3</c:v>
+                  <c:v>135.80000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5381,8 +5390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D48A558-673B-4B1E-8FF7-FCB07FA6F0FA}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5412,7 +5421,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -5528,10 +5537,10 @@
         <v>8.5900000000000004E-2</v>
       </c>
       <c r="F11">
-        <v>1.418E-2</v>
+        <v>1.204E-2</v>
       </c>
       <c r="G11">
-        <v>1.418E-2</v>
+        <v>1.1679999999999999E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -5551,10 +5560,10 @@
         <v>0.11609999999999999</v>
       </c>
       <c r="F12">
-        <v>2.2919999999999999E-2</v>
+        <v>1.9449999999999999E-2</v>
       </c>
       <c r="G12">
-        <v>2.248E-2</v>
+        <v>1.882E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -5574,10 +5583,10 @@
         <v>0.15129999999999999</v>
       </c>
       <c r="F13">
-        <v>3.4250000000000003E-2</v>
+        <v>3.006E-2</v>
       </c>
       <c r="G13">
-        <v>3.2559999999999999E-2</v>
+        <v>2.819E-2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -5594,10 +5603,10 @@
         <v>0.19400000000000001</v>
       </c>
       <c r="F14">
-        <v>4.8520000000000001E-2</v>
+        <v>4.2819999999999997E-2</v>
       </c>
       <c r="G14">
-        <v>4.7539999999999999E-2</v>
+        <v>4.1300000000000003E-2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -5614,10 +5623,10 @@
         <v>0.2422</v>
       </c>
       <c r="F15">
-        <v>6.5379999999999994E-2</v>
+        <v>5.7709999999999997E-2</v>
       </c>
       <c r="G15">
-        <v>6.4579999999999999E-2</v>
+        <v>5.7270000000000001E-2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -5634,10 +5643,10 @@
         <v>0.29699999999999999</v>
       </c>
       <c r="F16">
-        <v>8.5089999999999999E-2</v>
+        <v>7.6439999999999994E-2</v>
       </c>
       <c r="G16">
-        <v>8.5269999999999999E-2</v>
+        <v>7.671E-2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -5654,10 +5663,10 @@
         <v>0.36520000000000002</v>
       </c>
       <c r="F17">
-        <v>0.11310000000000001</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="G17">
-        <v>0.1119</v>
+        <v>0.10349999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -5674,10 +5683,10 @@
         <v>0.43440000000000001</v>
       </c>
       <c r="F18">
-        <v>0.1457</v>
+        <v>0.13289999999999999</v>
       </c>
       <c r="G18">
-        <v>0.1474</v>
+        <v>0.1366</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -5694,10 +5703,10 @@
         <v>0.5151</v>
       </c>
       <c r="F19">
-        <v>0.17899999999999999</v>
+        <v>0.1643</v>
       </c>
       <c r="G19">
-        <v>0.1918</v>
+        <v>0.1804</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -5714,10 +5723,10 @@
         <v>0.60899999999999999</v>
       </c>
       <c r="F20">
-        <v>0.22489999999999999</v>
+        <v>0.20669999999999999</v>
       </c>
       <c r="G20">
-        <v>0.24129999999999999</v>
+        <v>0.22650000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -5734,10 +5743,10 @@
         <v>0.70930000000000004</v>
       </c>
       <c r="F21">
-        <v>0.28120000000000001</v>
+        <v>0.25790000000000002</v>
       </c>
       <c r="G21">
-        <v>0.30509999999999998</v>
+        <v>0.28560000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -5754,10 +5763,10 @@
         <v>0.82320000000000004</v>
       </c>
       <c r="F22">
-        <v>0.34720000000000001</v>
+        <v>0.31940000000000002</v>
       </c>
       <c r="G22">
-        <v>0.3846</v>
+        <v>0.36120000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -5774,10 +5783,10 @@
         <v>0.94620000000000004</v>
       </c>
       <c r="F23">
-        <v>0.42899999999999999</v>
+        <v>0.39550000000000002</v>
       </c>
       <c r="G23">
-        <v>0.4824</v>
+        <v>0.45379999999999998</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -5794,10 +5803,10 @@
         <v>1.08</v>
       </c>
       <c r="F24">
-        <v>0.52859999999999996</v>
+        <v>0.49099999999999999</v>
       </c>
       <c r="G24">
-        <v>0.59799999999999998</v>
+        <v>0.56469999999999998</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -5814,10 +5823,10 @@
         <v>1.238</v>
       </c>
       <c r="F25">
-        <v>0.6462</v>
+        <v>0.60060000000000002</v>
       </c>
       <c r="G25">
-        <v>0.73080000000000001</v>
+        <v>0.69489999999999996</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -5834,10 +5843,10 @@
         <v>1.4179999999999999</v>
       </c>
       <c r="F26">
-        <v>0.79359999999999997</v>
+        <v>0.74009999999999998</v>
       </c>
       <c r="G26">
-        <v>0.88729999999999998</v>
+        <v>0.8458</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -5854,10 +5863,10 @@
         <v>1.617</v>
       </c>
       <c r="F27">
-        <v>0.96650000000000003</v>
+        <v>0.90049999999999997</v>
       </c>
       <c r="G27">
-        <v>1.0649999999999999</v>
+        <v>1.018</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -5874,10 +5883,10 @@
         <v>1.83</v>
       </c>
       <c r="F28">
-        <v>1.18</v>
+        <v>1.095</v>
       </c>
       <c r="G28">
-        <v>1.26</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -5894,10 +5903,10 @@
         <v>2.0739999999999998</v>
       </c>
       <c r="F29">
-        <v>1.4330000000000001</v>
+        <v>1.33</v>
       </c>
       <c r="G29">
-        <v>1.4990000000000001</v>
+        <v>1.45</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -5914,10 +5923,10 @@
         <v>2.3559999999999999</v>
       </c>
       <c r="F30">
-        <v>1.742</v>
+        <v>1.6080000000000001</v>
       </c>
       <c r="G30">
-        <v>1.7669999999999999</v>
+        <v>1.7170000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -5934,10 +5943,10 @@
         <v>2.6779999999999999</v>
       </c>
       <c r="F31">
-        <v>2.1269999999999998</v>
+        <v>1.954</v>
       </c>
       <c r="G31">
-        <v>2.073</v>
+        <v>2.0179999999999998</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -5954,10 +5963,10 @@
         <v>3.036</v>
       </c>
       <c r="F32">
-        <v>2.6160000000000001</v>
+        <v>2.3690000000000002</v>
       </c>
       <c r="G32">
-        <v>2.407</v>
+        <v>2.355</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -5974,10 +5983,10 @@
         <v>3.4319999999999999</v>
       </c>
       <c r="F33">
-        <v>3.2490000000000001</v>
+        <v>2.8860000000000001</v>
       </c>
       <c r="G33">
-        <v>2.762</v>
+        <v>2.7170000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -5994,10 +6003,10 @@
         <v>3.8820000000000001</v>
       </c>
       <c r="F34">
-        <v>4.1619999999999999</v>
+        <v>3.544</v>
       </c>
       <c r="G34">
-        <v>3.2360000000000002</v>
+        <v>3.1949999999999998</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -6014,10 +6023,10 @@
         <v>4.3789999999999996</v>
       </c>
       <c r="F35">
-        <v>5.5209999999999999</v>
+        <v>4.3579999999999997</v>
       </c>
       <c r="G35">
-        <v>3.6869999999999998</v>
+        <v>3.6389999999999998</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -6034,10 +6043,10 @@
         <v>4.9329999999999998</v>
       </c>
       <c r="F36">
-        <v>8.0180000000000007</v>
+        <v>5.3819999999999997</v>
       </c>
       <c r="G36">
-        <v>4.2089999999999996</v>
+        <v>4.1580000000000004</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -6053,8 +6062,11 @@
       <c r="E37">
         <v>5.5570000000000004</v>
       </c>
+      <c r="F37">
+        <v>6.9409999999999998</v>
+      </c>
       <c r="G37">
-        <v>4.8659999999999997</v>
+        <v>4.7910000000000004</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -6070,8 +6082,11 @@
       <c r="E38">
         <v>6.2430000000000003</v>
       </c>
+      <c r="F38">
+        <v>9.1479999999999997</v>
+      </c>
       <c r="G38">
-        <v>5.5049999999999999</v>
+        <v>5.431</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -6088,7 +6103,7 @@
         <v>7.0279999999999996</v>
       </c>
       <c r="G39">
-        <v>6.2610000000000001</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -6105,7 +6120,7 @@
         <v>7.9009999999999998</v>
       </c>
       <c r="G40">
-        <v>7.157</v>
+        <v>7.0449999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -6122,7 +6137,7 @@
         <v>8.85</v>
       </c>
       <c r="G41">
-        <v>8.0990000000000002</v>
+        <v>7.9409999999999998</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -6139,7 +6154,7 @@
         <v>9.9809999999999999</v>
       </c>
       <c r="G42">
-        <v>9.2430000000000003</v>
+        <v>9.0619999999999994</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -6166,10 +6181,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD5C0124-FDAB-4252-836F-9CFDB475E886}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6195,7 +6210,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>
@@ -6263,12 +6278,6 @@
       <c r="E7">
         <v>5.985E-2</v>
       </c>
-      <c r="F7">
-        <v>1.1950000000000001E-2</v>
-      </c>
-      <c r="G7">
-        <v>1.044E-2</v>
-      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -6284,10 +6293,7 @@
         <v>7.7600000000000002E-2</v>
       </c>
       <c r="F8">
-        <v>2.069E-2</v>
-      </c>
-      <c r="G8">
-        <v>1.7659999999999999E-2</v>
+        <v>1.204E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -6304,10 +6310,10 @@
         <v>9.8390000000000005E-2</v>
       </c>
       <c r="F9">
-        <v>3.175E-2</v>
+        <v>1.9449999999999999E-2</v>
       </c>
       <c r="G9">
-        <v>2.7650000000000001E-2</v>
+        <v>1.686E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -6324,10 +6330,10 @@
         <v>0.122</v>
       </c>
       <c r="F10">
-        <v>5.058E-2</v>
+        <v>3.4520000000000002E-2</v>
       </c>
       <c r="G10">
-        <v>4.0320000000000002E-2</v>
+        <v>2.605E-2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -6344,10 +6350,10 @@
         <v>0.15409999999999999</v>
       </c>
       <c r="F11">
-        <v>7.9740000000000005E-2</v>
+        <v>6.1100000000000002E-2</v>
       </c>
       <c r="G11">
-        <v>6.164E-2</v>
+        <v>4.326E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -6364,10 +6370,10 @@
         <v>0.1905</v>
       </c>
       <c r="F12">
-        <v>0.1229</v>
+        <v>0.1038</v>
       </c>
       <c r="G12">
-        <v>9.5170000000000005E-2</v>
+        <v>7.3230000000000003E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -6384,10 +6390,10 @@
         <v>0.2407</v>
       </c>
       <c r="F13">
-        <v>0.2031</v>
+        <v>0.186</v>
       </c>
       <c r="G13">
-        <v>0.1409</v>
+        <v>0.1168</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -6404,10 +6410,10 @@
         <v>0.30919999999999997</v>
       </c>
       <c r="F14">
-        <v>0.32400000000000001</v>
+        <v>0.31140000000000001</v>
       </c>
       <c r="G14">
-        <v>0.20050000000000001</v>
+        <v>0.1754</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -6424,10 +6430,10 @@
         <v>0.39729999999999999</v>
       </c>
       <c r="F15">
-        <v>0.50919999999999999</v>
+        <v>0.4768</v>
       </c>
       <c r="G15">
-        <v>0.2903</v>
+        <v>0.26600000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -6444,10 +6450,10 @@
         <v>0.5242</v>
       </c>
       <c r="F16">
-        <v>0.78349999999999997</v>
+        <v>0.73850000000000005</v>
       </c>
       <c r="G16">
-        <v>0.41060000000000002</v>
+        <v>0.38579999999999998</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -6464,10 +6470,10 @@
         <v>0.68600000000000005</v>
       </c>
       <c r="F17">
-        <v>1.1950000000000001</v>
+        <v>1.0840000000000001</v>
       </c>
       <c r="G17">
-        <v>0.57069999999999999</v>
+        <v>0.54569999999999996</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -6484,10 +6490,10 @@
         <v>0.8881</v>
       </c>
       <c r="F18">
-        <v>1.8320000000000001</v>
+        <v>1.5720000000000001</v>
       </c>
       <c r="G18">
-        <v>0.76549999999999996</v>
+        <v>0.74450000000000005</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -6504,10 +6510,10 @@
         <v>1.147</v>
       </c>
       <c r="F19">
-        <v>2.911</v>
+        <v>2.294</v>
       </c>
       <c r="G19">
-        <v>1.004</v>
+        <v>0.98280000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -6524,10 +6530,10 @@
         <v>1.46</v>
       </c>
       <c r="F20">
-        <v>5.0650000000000004</v>
+        <v>3.2949999999999999</v>
       </c>
       <c r="G20">
-        <v>1.2849999999999999</v>
+        <v>1.2669999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -6544,10 +6550,10 @@
         <v>1.841</v>
       </c>
       <c r="F21">
-        <v>22.65</v>
+        <v>4.8680000000000003</v>
       </c>
       <c r="G21">
-        <v>1.643</v>
+        <v>1.625</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -6563,8 +6569,11 @@
       <c r="E22">
         <v>2.2999999999999998</v>
       </c>
+      <c r="F22">
+        <v>7.5640000000000001</v>
+      </c>
       <c r="G22">
-        <v>2.097</v>
+        <v>2.08</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -6580,8 +6589,11 @@
       <c r="E23">
         <v>2.819</v>
       </c>
+      <c r="F23">
+        <v>13.13</v>
+      </c>
       <c r="G23">
-        <v>2.6379999999999999</v>
+        <v>2.61</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -6597,8 +6609,11 @@
       <c r="E24">
         <v>3.4220000000000002</v>
       </c>
+      <c r="F24">
+        <v>56.99</v>
+      </c>
       <c r="G24">
-        <v>3.2290000000000001</v>
+        <v>3.165</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -6615,7 +6630,7 @@
         <v>4.1360000000000001</v>
       </c>
       <c r="G25">
-        <v>3.9580000000000002</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -6632,7 +6647,7 @@
         <v>4.944</v>
       </c>
       <c r="G26">
-        <v>4.8739999999999997</v>
+        <v>4.7370000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -6649,7 +6664,7 @@
         <v>5.8440000000000003</v>
       </c>
       <c r="G27">
-        <v>5.8250000000000002</v>
+        <v>5.6870000000000003</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -6666,7 +6681,7 @@
         <v>6.8609999999999998</v>
       </c>
       <c r="G28">
-        <v>7.1609999999999996</v>
+        <v>6.9249999999999998</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -6683,7 +6698,7 @@
         <v>7.9749999999999996</v>
       </c>
       <c r="G29">
-        <v>8.6920000000000002</v>
+        <v>8.1839999999999993</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -6700,7 +6715,7 @@
         <v>9.1880000000000006</v>
       </c>
       <c r="G30">
-        <v>10.39</v>
+        <v>9.8940000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -6714,7 +6729,7 @@
         <v>2.9729999999999999</v>
       </c>
       <c r="G31">
-        <v>12.63</v>
+        <v>11.57</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -6728,7 +6743,7 @@
         <v>3.3010000000000002</v>
       </c>
       <c r="G32">
-        <v>14.92</v>
+        <v>13.95</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -6742,7 +6757,7 @@
         <v>3.6440000000000001</v>
       </c>
       <c r="G33">
-        <v>18.25</v>
+        <v>16.43</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -6756,7 +6771,7 @@
         <v>4.0289999999999999</v>
       </c>
       <c r="G34">
-        <v>22.1</v>
+        <v>19.670000000000002</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -6770,7 +6785,7 @@
         <v>4.4219999999999997</v>
       </c>
       <c r="G35">
-        <v>26.81</v>
+        <v>23.36</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -6784,7 +6799,7 @@
         <v>4.8380000000000001</v>
       </c>
       <c r="G36">
-        <v>32.94</v>
+        <v>27.85</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -6798,7 +6813,7 @@
         <v>5.2830000000000004</v>
       </c>
       <c r="G37">
-        <v>40.25</v>
+        <v>33.39</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -6809,7 +6824,7 @@
         <v>5.7839999999999998</v>
       </c>
       <c r="G38">
-        <v>50.01</v>
+        <v>39.96</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -6820,7 +6835,7 @@
         <v>6.3049999999999997</v>
       </c>
       <c r="G39">
-        <v>62.46</v>
+        <v>48.32</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -6831,7 +6846,7 @@
         <v>6.8719999999999999</v>
       </c>
       <c r="G40">
-        <v>79.41</v>
+        <v>58.22</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -6842,7 +6857,7 @@
         <v>7.49</v>
       </c>
       <c r="G41">
-        <v>101.9</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -6853,7 +6868,7 @@
         <v>8.1359999999999992</v>
       </c>
       <c r="G42">
-        <v>133</v>
+        <v>87.23</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -6864,7 +6879,7 @@
         <v>8.8119999999999994</v>
       </c>
       <c r="G43">
-        <v>179.5</v>
+        <v>108.7</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -6875,12 +6890,37 @@
         <v>9.5589999999999993</v>
       </c>
       <c r="G44">
-        <v>251.3</v>
+        <v>135.80000000000001</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G45">
-        <v>603.79999999999995</v>
+        <v>171.9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G46">
+        <v>222.8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G47">
+        <v>293.39999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G48">
+        <v>393.6</v>
+      </c>
+    </row>
+    <row r="49" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G49">
+        <v>560.20000000000005</v>
+      </c>
+    </row>
+    <row r="50" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G50">
+        <v>914.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>